<commit_message>
remove xsl sheet not needed
</commit_message>
<xml_diff>
--- a/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
+++ b/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k.weheliye/Desktop/tarabut/compliance/leecode-java/src/main/java/org/code/challenges/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A525DC28-5F8F-3A4E-8F3B-AE464B9EBB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A28CF2-0C6B-184A-A517-1AE9DA6727BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="326">
   <si>
     <t>Video Solution</t>
   </si>
@@ -996,6 +996,9 @@
   </si>
   <si>
     <t>Is Subsequence</t>
+  </si>
+  <si>
+    <t>Two Pointers: We can use two pointers to solve this in linear time. If we find that s[i] == t[j], that means we "found" the letter at position i for s, and we can move on to the next one by incrementing i.</t>
   </si>
 </sst>
 </file>
@@ -1278,7 +1281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1306,8 +1309,6 @@
     <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1527,7 +1528,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1594,14 +1595,17 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="24" t="s">
         <v>324</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>323</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -1642,7 +1646,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1659,7 +1663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1680,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -1693,7 +1697,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
@@ -1710,7 +1714,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
@@ -1727,7 +1731,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
@@ -1744,7 +1748,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>26</v>
       </c>
@@ -1761,7 +1765,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>30</v>
       </c>
@@ -1778,7 +1782,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>34</v>
       </c>
@@ -1795,7 +1799,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>38</v>
       </c>
@@ -1812,7 +1816,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>42</v>
       </c>
@@ -1829,7 +1833,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>46</v>
       </c>
@@ -1846,7 +1850,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>51</v>
       </c>
@@ -1863,7 +1867,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>55</v>
       </c>
@@ -1880,7 +1884,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>59</v>
       </c>
@@ -1897,7 +1901,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>63</v>
       </c>
@@ -1914,7 +1918,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>67</v>
       </c>
@@ -1931,7 +1935,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>72</v>
       </c>
@@ -1948,7 +1952,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>76</v>
       </c>
@@ -1965,7 +1969,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>80</v>
       </c>
@@ -1982,7 +1986,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>84</v>
       </c>
@@ -1999,7 +2003,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>88</v>
       </c>
@@ -2016,7 +2020,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>92</v>
       </c>
@@ -2033,7 +2037,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>96</v>
       </c>
@@ -2050,7 +2054,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>100</v>
       </c>
@@ -2067,7 +2071,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>104</v>
       </c>
@@ -2084,7 +2088,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>108</v>
       </c>
@@ -2101,7 +2105,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>112</v>
       </c>
@@ -2118,7 +2122,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>117</v>
       </c>
@@ -2135,7 +2139,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>121</v>
       </c>
@@ -2152,7 +2156,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>125</v>
       </c>
@@ -2169,7 +2173,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>129</v>
       </c>
@@ -2186,7 +2190,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>133</v>
       </c>
@@ -2203,7 +2207,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>137</v>
       </c>
@@ -2220,7 +2224,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>141</v>
       </c>
@@ -2237,7 +2241,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>145</v>
       </c>
@@ -2254,7 +2258,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>150</v>
       </c>
@@ -2271,7 +2275,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>154</v>
       </c>
@@ -2288,7 +2292,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>158</v>
       </c>
@@ -2305,7 +2309,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="s">
         <v>162</v>
       </c>
@@ -2322,7 +2326,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>166</v>
       </c>
@@ -2339,7 +2343,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>171</v>
       </c>
@@ -2356,7 +2360,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>175</v>
       </c>
@@ -2373,7 +2377,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>179</v>
       </c>
@@ -2390,7 +2394,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>183</v>
       </c>
@@ -2407,7 +2411,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>187</v>
       </c>
@@ -2424,7 +2428,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>191</v>
       </c>
@@ -2441,7 +2445,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>196</v>
       </c>

</xml_diff>

<commit_message>
Sum longest SubbArray challenge
</commit_message>
<xml_diff>
--- a/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
+++ b/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k.weheliye/Desktop/tarabut/compliance/leecode-java/src/main/java/org/code/challenges/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F579CCE-5BF1-164E-9F40-BDF07324030B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94BFD10-EACF-E74A-96D7-223332B9EC66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="760" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Category</t>
   </si>
@@ -89,13 +89,54 @@
   </si>
   <si>
     <t xml:space="preserve">Two Pointers: create third variable (index) that equals last index of array and decrement </t>
+  </si>
+  <si>
+    <t>Technique</t>
+  </si>
+  <si>
+    <t>Two pointers</t>
+  </si>
+  <si>
+    <t>Two Pointers</t>
+  </si>
+  <si>
+    <t>Sum SubString SubArray</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t>Slide Window</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,Two Pointers, Sub Array</t>
+    </r>
+  </si>
+  <si>
+    <t>Slide window: add element to slide-window and remove it based on the constraint , use loop to remove element from slide-window</t>
+  </si>
+  <si>
+    <t>Sum Longest SubArray</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -129,8 +170,20 @@
       <color rgb="FF000000"/>
       <name val="Arial (Body)"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial (Body)"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,6 +193,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -185,7 +244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -193,6 +252,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -409,20 +471,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13703DB-FEA8-9246-9D4D-5D4B2C6A9445}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" customWidth="1"/>
     <col min="3" max="3" width="53.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.1640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,11 +495,14 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -447,10 +513,13 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -461,10 +530,13 @@
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -474,11 +546,14 @@
       <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -488,11 +563,14 @@
       <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -502,11 +580,14 @@
       <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -516,8 +597,39 @@
       <c r="C7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prefix sum without array only'varibale'
</commit_message>
<xml_diff>
--- a/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
+++ b/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamal/Documents/yallafix/leecode-java/src/main/java/org/code/challenges/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39F20B5-A868-384C-8977-7ED5907E4D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D965CB2-C936-2D48-BC07-C12B88779DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="540" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
   <si>
     <t>Category</t>
   </si>
@@ -426,13 +426,51 @@
   </si>
   <si>
     <t>Max Consecutive Ones III</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Number of Ways to Split Array (With Array)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-ways-to-split-array/</t>
+  </si>
+  <si>
+    <t>Prefix Sum</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Prefix Sum: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t>use an array to calculate the prefix of all sum elements</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> Number of Ways to Split Array (Without Array)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Prefix Sum: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t>use a variable instead of array  to calculate the prefix of all sum elements</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -465,13 +503,6 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial (Body)"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
@@ -565,10 +596,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -785,18 +816,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13703DB-FEA8-9246-9D4D-5D4B2C6A9445}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="76.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.83203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -816,7 +847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -833,7 +864,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -850,7 +881,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -867,7 +898,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -884,7 +915,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -901,7 +932,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -918,11 +949,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -932,11 +963,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -946,11 +977,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -963,25 +994,25 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -990,15 +1021,15 @@
       <c r="D12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -1007,8 +1038,42 @@
       <c r="D13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1022,6 +1087,8 @@
     <hyperlink ref="C10" r:id="rId7" xr:uid="{F7F388A7-ACD1-E140-B119-D7BCFD50F5FE}"/>
     <hyperlink ref="C12" r:id="rId8" xr:uid="{77A7E089-AC14-AB4A-B671-C0D310CB6CF3}"/>
     <hyperlink ref="C13" r:id="rId9" xr:uid="{BCDCDE6F-1466-074A-BB9F-F0CB675CA923}"/>
+    <hyperlink ref="C14" r:id="rId10" xr:uid="{0C111F3E-212C-5649-8472-D8D2118553C9}"/>
+    <hyperlink ref="C15" r:id="rId11" xr:uid="{FA8897B0-989F-4843-8C79-077B8E564DE2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
1480: Running Sum of 1d Array
</commit_message>
<xml_diff>
--- a/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
+++ b/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamal/Documents/yallafix/leecode-java/src/main/java/org/code/challenges/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D965CB2-C936-2D48-BC07-C12B88779DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66CF4B5-FDA0-3845-8DCE-CAFDC3C1B3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
   <si>
     <t>Category</t>
   </si>
@@ -428,9 +428,6 @@
     <t>Max Consecutive Ones III</t>
   </si>
   <si>
-    <t xml:space="preserve"> Number of Ways to Split Array (With Array)</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/number-of-ways-to-split-array/</t>
   </si>
   <si>
@@ -450,9 +447,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> Number of Ways to Split Array (Without Array)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Prefix Sum: </t>
     </r>
@@ -464,6 +458,50 @@
       </rPr>
       <t>use a variable instead of array  to calculate the prefix of all sum elements</t>
     </r>
+  </si>
+  <si>
+    <t>Running Sum of 1d Array</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/running-sum-of-1d-array/</t>
+  </si>
+  <si>
+    <t>Using Separate Array, Using Input Array for Output</t>
+  </si>
+  <si>
+    <r>
+      <t>Their's two approach to solve this challenge , either create a seprate array to store sum of elements (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t>result[i] = result[i - 1] + nums[i]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t>;) , or use same input array for return output</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> (nums[i] += nums[i - 1];)</t>
+    </r>
+  </si>
+  <si>
+    <t>Number of Ways to Split Array (Without Array)</t>
+  </si>
+  <si>
+    <t>Number of Ways to Split Array (With Array)</t>
   </si>
 </sst>
 </file>
@@ -816,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13703DB-FEA8-9246-9D4D-5D4B2C6A9445}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -937,30 +975,33 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>28</v>
+      <c r="B8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -968,10 +1009,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>27</v>
@@ -982,16 +1023,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -999,13 +1037,16 @@
         <v>4</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>35</v>
+        <v>29</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1013,33 +1054,30 @@
         <v>4</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>43</v>
+        <v>32</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1047,33 +1085,50 @@
         <v>40</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>47</v>
+        <v>41</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D15" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>50</v>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1083,12 +1138,13 @@
     <hyperlink ref="C4" r:id="rId3" xr:uid="{6B9C3297-C807-CF43-AA7B-E97378371948}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{2A0E9DC2-E8F4-764A-989D-FBB9493AF002}"/>
     <hyperlink ref="C6" r:id="rId5" xr:uid="{C9094BB3-3FEE-B44C-A115-D650C9CB57A5}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{B9BEF090-2AFE-9441-AD50-35C1A5966885}"/>
-    <hyperlink ref="C10" r:id="rId7" xr:uid="{F7F388A7-ACD1-E140-B119-D7BCFD50F5FE}"/>
-    <hyperlink ref="C12" r:id="rId8" xr:uid="{77A7E089-AC14-AB4A-B671-C0D310CB6CF3}"/>
-    <hyperlink ref="C13" r:id="rId9" xr:uid="{BCDCDE6F-1466-074A-BB9F-F0CB675CA923}"/>
-    <hyperlink ref="C14" r:id="rId10" xr:uid="{0C111F3E-212C-5649-8472-D8D2118553C9}"/>
-    <hyperlink ref="C15" r:id="rId11" xr:uid="{FA8897B0-989F-4843-8C79-077B8E564DE2}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{B9BEF090-2AFE-9441-AD50-35C1A5966885}"/>
+    <hyperlink ref="C11" r:id="rId7" xr:uid="{F7F388A7-ACD1-E140-B119-D7BCFD50F5FE}"/>
+    <hyperlink ref="C13" r:id="rId8" xr:uid="{77A7E089-AC14-AB4A-B671-C0D310CB6CF3}"/>
+    <hyperlink ref="C14" r:id="rId9" xr:uid="{BCDCDE6F-1466-074A-BB9F-F0CB675CA923}"/>
+    <hyperlink ref="C15" r:id="rId10" xr:uid="{0C111F3E-212C-5649-8472-D8D2118553C9}"/>
+    <hyperlink ref="C16" r:id="rId11" xr:uid="{FA8897B0-989F-4843-8C79-077B8E564DE2}"/>
+    <hyperlink ref="C7" r:id="rId12" xr:uid="{1ED9A352-B7B9-AB40-B432-CF109BDAF648}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
1413. Minimum Value to Get Positive Step by Step Sum
</commit_message>
<xml_diff>
--- a/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
+++ b/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamal/Documents/yallafix/leecode-java/src/main/java/org/code/challenges/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66CF4B5-FDA0-3845-8DCE-CAFDC3C1B3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD8784B-7FC5-8741-9294-A51F715CCC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
   <si>
     <t>Category</t>
-  </si>
-  <si>
-    <t>Name</t>
   </si>
   <si>
     <t>Link</t>
@@ -502,6 +499,58 @@
   </si>
   <si>
     <t>Number of Ways to Split Array (With Array)</t>
+  </si>
+  <si>
+    <t>Class name</t>
+  </si>
+  <si>
+    <t>Challenge Name</t>
+  </si>
+  <si>
+    <t>Minimum Value to Get Positive Step by Step Sum</t>
+  </si>
+  <si>
+    <t>MinimumValueToGetPositiveStepByStepSum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-value-to-get-positive-step-by-step-sum/</t>
+  </si>
+  <si>
+    <r>
+      <t>Use</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> PrefixSum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> Technique and get minimum prefix value </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve">Math.min(minPrefixSum, sum), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve">then </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -626,7 +675,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -638,6 +687,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -854,281 +906,320 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13703DB-FEA8-9246-9D4D-5D4B2C6A9445}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="48.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="76.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.6640625" customWidth="1"/>
+    <col min="3" max="3" width="63.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.1640625" customWidth="1"/>
+    <col min="5" max="5" width="76.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="255.83203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="F9" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="7" t="s">
+      <c r="D16" s="3"/>
+      <c r="E16" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="9" t="s">
+      <c r="F17" s="9" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1138,13 +1229,14 @@
     <hyperlink ref="C4" r:id="rId3" xr:uid="{6B9C3297-C807-CF43-AA7B-E97378371948}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{2A0E9DC2-E8F4-764A-989D-FBB9493AF002}"/>
     <hyperlink ref="C6" r:id="rId5" xr:uid="{C9094BB3-3FEE-B44C-A115-D650C9CB57A5}"/>
-    <hyperlink ref="C8" r:id="rId6" xr:uid="{B9BEF090-2AFE-9441-AD50-35C1A5966885}"/>
-    <hyperlink ref="C11" r:id="rId7" xr:uid="{F7F388A7-ACD1-E140-B119-D7BCFD50F5FE}"/>
-    <hyperlink ref="C13" r:id="rId8" xr:uid="{77A7E089-AC14-AB4A-B671-C0D310CB6CF3}"/>
-    <hyperlink ref="C14" r:id="rId9" xr:uid="{BCDCDE6F-1466-074A-BB9F-F0CB675CA923}"/>
-    <hyperlink ref="C15" r:id="rId10" xr:uid="{0C111F3E-212C-5649-8472-D8D2118553C9}"/>
-    <hyperlink ref="C16" r:id="rId11" xr:uid="{FA8897B0-989F-4843-8C79-077B8E564DE2}"/>
+    <hyperlink ref="C9" r:id="rId6" xr:uid="{B9BEF090-2AFE-9441-AD50-35C1A5966885}"/>
+    <hyperlink ref="C12" r:id="rId7" xr:uid="{F7F388A7-ACD1-E140-B119-D7BCFD50F5FE}"/>
+    <hyperlink ref="C14" r:id="rId8" xr:uid="{77A7E089-AC14-AB4A-B671-C0D310CB6CF3}"/>
+    <hyperlink ref="C15" r:id="rId9" xr:uid="{BCDCDE6F-1466-074A-BB9F-F0CB675CA923}"/>
+    <hyperlink ref="C16" r:id="rId10" xr:uid="{0C111F3E-212C-5649-8472-D8D2118553C9}"/>
+    <hyperlink ref="C17" r:id="rId11" xr:uid="{FA8897B0-989F-4843-8C79-077B8E564DE2}"/>
     <hyperlink ref="C7" r:id="rId12" xr:uid="{1ED9A352-B7B9-AB40-B432-CF109BDAF648}"/>
+    <hyperlink ref="C8" r:id="rId13" xr:uid="{AAA3065A-A5DD-DA4B-B0C7-BB17201B4434}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
1413. Minimum Value to Get Positive Step by Step Sum  Brute Force Solution
</commit_message>
<xml_diff>
--- a/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
+++ b/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamal/Documents/yallafix/leecode-java/src/main/java/org/code/challenges/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD8784B-7FC5-8741-9294-A51F715CCC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11757F54-AE9A-344A-B85B-9BAF82CC7012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -510,9 +510,6 @@
     <t>Minimum Value to Get Positive Step by Step Sum</t>
   </si>
   <si>
-    <t>MinimumValueToGetPositiveStepByStepSum</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/minimum-value-to-get-positive-step-by-step-sum/</t>
   </si>
   <si>
@@ -551,6 +548,9 @@
       </rPr>
       <t xml:space="preserve">then </t>
     </r>
+  </si>
+  <si>
+    <t>MinimumValueToGetPositiveStepByStepSum_Prefix</t>
   </si>
 </sst>
 </file>
@@ -908,15 +908,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13703DB-FEA8-9246-9D4D-5D4B2C6A9445}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="54.6640625" customWidth="1"/>
     <col min="3" max="3" width="63.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.1640625" customWidth="1"/>
+    <col min="4" max="4" width="60.6640625" customWidth="1"/>
     <col min="5" max="5" width="76.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="255.83203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
@@ -1057,16 +1057,16 @@
         <v>56</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>45</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
K Radius Subarray Averages
</commit_message>
<xml_diff>
--- a/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
+++ b/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamal/Documents/yallafix/leecode-java/src/main/java/org/code/challenges/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74D3CAC-D814-AE49-936C-31B7A25013C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230E3834-7E88-BA4D-8CAC-FE2431922ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
   <si>
     <t>Category</t>
   </si>
@@ -578,6 +578,18 @@
       </rPr>
       <t>break from the while loop</t>
     </r>
+  </si>
+  <si>
+    <t>K Radius Subarray Averages (Prefix)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/k-radius-subarray-averages/</t>
+  </si>
+  <si>
+    <t>KRadiusSubarrayAverages_PrefixSolution</t>
+  </si>
+  <si>
+    <t>Prefix Sum:</t>
   </si>
 </sst>
 </file>
@@ -702,7 +714,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -715,6 +727,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -933,17 +948,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13703DB-FEA8-9246-9D4D-5D4B2C6A9445}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="54.6640625" customWidth="1"/>
     <col min="3" max="3" width="63.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.5" customWidth="1"/>
+    <col min="4" max="4" width="65.5" style="3" customWidth="1"/>
     <col min="5" max="5" width="76.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="255.83203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
@@ -978,7 +993,6 @@
       <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
         <v>23</v>
       </c>
@@ -996,7 +1010,6 @@
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
         <v>23</v>
       </c>
@@ -1014,7 +1027,6 @@
       <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
         <v>23</v>
       </c>
@@ -1032,7 +1044,6 @@
       <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
         <v>23</v>
       </c>
@@ -1050,7 +1061,6 @@
       <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
         <v>23</v>
       </c>
@@ -1068,7 +1078,6 @@
       <c r="C7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
         <v>50</v>
       </c>
@@ -1126,7 +1135,6 @@
       <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
         <v>24</v>
       </c>
@@ -1141,7 +1149,6 @@
       <c r="B11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
         <v>32</v>
       </c>
@@ -1156,7 +1163,6 @@
       <c r="B12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
         <v>33</v>
       </c>
@@ -1174,7 +1180,6 @@
       <c r="C13" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
         <v>33</v>
       </c>
@@ -1189,7 +1194,6 @@
       <c r="B14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
         <v>31</v>
       </c>
@@ -1207,7 +1211,6 @@
       <c r="C15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
         <v>31</v>
       </c>
@@ -1225,7 +1228,6 @@
       <c r="C16" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
         <v>41</v>
       </c>
@@ -1243,7 +1245,6 @@
       <c r="C17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="3"/>
       <c r="E17" s="10" t="s">
         <v>45</v>
       </c>
@@ -1261,12 +1262,31 @@
       <c r="C18" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="3"/>
       <c r="E18" s="10" t="s">
         <v>45</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1284,6 +1304,7 @@
     <hyperlink ref="C18" r:id="rId11" xr:uid="{FA8897B0-989F-4843-8C79-077B8E564DE2}"/>
     <hyperlink ref="C7" r:id="rId12" xr:uid="{1ED9A352-B7B9-AB40-B432-CF109BDAF648}"/>
     <hyperlink ref="C9" r:id="rId13" xr:uid="{AAA3065A-A5DD-DA4B-B0C7-BB17201B4434}"/>
+    <hyperlink ref="C19" r:id="rId14" xr:uid="{6A8EE19C-D739-2B4C-A65D-8F9DF01F42D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added new way to solve it
</commit_message>
<xml_diff>
--- a/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
+++ b/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamal/Documents/yallafix/leecode-java/src/main/java/org/code/challenges/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230E3834-7E88-BA4D-8CAC-FE2431922ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A7D262-6415-A944-A99D-C508772BB351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -589,7 +589,17 @@
     <t>KRadiusSubarrayAverages_PrefixSolution</t>
   </si>
   <si>
-    <t>Prefix Sum:</t>
+    <r>
+      <t>Prefix Sum:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> Check first if nums has K on left and right , create average array and initialize with -1</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -950,7 +960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13703DB-FEA8-9246-9D4D-5D4B2C6A9445}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
reverse word in string solution traverse and reverse
</commit_message>
<xml_diff>
--- a/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
+++ b/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamal/Documents/yallafix/leecode-java/src/main/java/org/code/challenges/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A7D262-6415-A944-A99D-C508772BB351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B14F95-64AF-4D49-A4E8-D8BBB9AA2B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
   <si>
     <t>Category</t>
   </si>
@@ -599,6 +599,66 @@
         <rFont val="Arial (Body)"/>
       </rPr>
       <t xml:space="preserve"> Check first if nums has K on left and right , create average array and initialize with -1</t>
+    </r>
+  </si>
+  <si>
+    <t>Reverse Words in a String III</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-words-in-a-string-iii</t>
+  </si>
+  <si>
+    <t>Traverse and Reverse each character one by one</t>
+  </si>
+  <si>
+    <t>ReverseWordsInAStringIII_TraverseReverse</t>
+  </si>
+  <si>
+    <t>RunningSumOf1dArray</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Their's only one edge case in here, the last word does not have a space after its last character, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t>you need two loop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t>loop one will iterate whole the string , and loop two will do reversing string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t>), of course you need and if statement to check whether their's space or is lastIndex</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> (if ((strIndex == s.length() - 1) || s.charAt(strIndex) == ' ')) </t>
     </r>
   </si>
 </sst>
@@ -958,10 +1018,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13703DB-FEA8-9246-9D4D-5D4B2C6A9445}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1083,36 +1143,39 @@
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="D8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.2">
@@ -1126,44 +1189,50 @@
         <v>57</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E10" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>27</v>
+      <c r="B11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1171,10 +1240,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>26</v>
@@ -1185,16 +1254,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1202,13 +1268,16 @@
         <v>3</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1216,33 +1285,30 @@
         <v>3</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>31</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>42</v>
+        <v>31</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1250,24 +1316,24 @@
         <v>39</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>44</v>
@@ -1276,26 +1342,43 @@
         <v>45</v>
       </c>
       <c r="F18" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="19" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="12" t="s">
+    <row r="20" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E20" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F20" s="8" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1306,15 +1389,16 @@
     <hyperlink ref="C4" r:id="rId3" xr:uid="{6B9C3297-C807-CF43-AA7B-E97378371948}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{2A0E9DC2-E8F4-764A-989D-FBB9493AF002}"/>
     <hyperlink ref="C6" r:id="rId5" xr:uid="{C9094BB3-3FEE-B44C-A115-D650C9CB57A5}"/>
-    <hyperlink ref="C10" r:id="rId6" xr:uid="{B9BEF090-2AFE-9441-AD50-35C1A5966885}"/>
-    <hyperlink ref="C13" r:id="rId7" xr:uid="{F7F388A7-ACD1-E140-B119-D7BCFD50F5FE}"/>
-    <hyperlink ref="C15" r:id="rId8" xr:uid="{77A7E089-AC14-AB4A-B671-C0D310CB6CF3}"/>
-    <hyperlink ref="C16" r:id="rId9" xr:uid="{BCDCDE6F-1466-074A-BB9F-F0CB675CA923}"/>
-    <hyperlink ref="C17" r:id="rId10" xr:uid="{0C111F3E-212C-5649-8472-D8D2118553C9}"/>
-    <hyperlink ref="C18" r:id="rId11" xr:uid="{FA8897B0-989F-4843-8C79-077B8E564DE2}"/>
-    <hyperlink ref="C7" r:id="rId12" xr:uid="{1ED9A352-B7B9-AB40-B432-CF109BDAF648}"/>
-    <hyperlink ref="C9" r:id="rId13" xr:uid="{AAA3065A-A5DD-DA4B-B0C7-BB17201B4434}"/>
-    <hyperlink ref="C19" r:id="rId14" xr:uid="{6A8EE19C-D739-2B4C-A65D-8F9DF01F42D6}"/>
+    <hyperlink ref="C11" r:id="rId6" xr:uid="{B9BEF090-2AFE-9441-AD50-35C1A5966885}"/>
+    <hyperlink ref="C14" r:id="rId7" xr:uid="{F7F388A7-ACD1-E140-B119-D7BCFD50F5FE}"/>
+    <hyperlink ref="C16" r:id="rId8" xr:uid="{77A7E089-AC14-AB4A-B671-C0D310CB6CF3}"/>
+    <hyperlink ref="C17" r:id="rId9" xr:uid="{BCDCDE6F-1466-074A-BB9F-F0CB675CA923}"/>
+    <hyperlink ref="C18" r:id="rId10" xr:uid="{0C111F3E-212C-5649-8472-D8D2118553C9}"/>
+    <hyperlink ref="C19" r:id="rId11" xr:uid="{FA8897B0-989F-4843-8C79-077B8E564DE2}"/>
+    <hyperlink ref="C8" r:id="rId12" xr:uid="{1ED9A352-B7B9-AB40-B432-CF109BDAF648}"/>
+    <hyperlink ref="C10" r:id="rId13" xr:uid="{AAA3065A-A5DD-DA4B-B0C7-BB17201B4434}"/>
+    <hyperlink ref="C20" r:id="rId14" xr:uid="{6A8EE19C-D739-2B4C-A65D-8F9DF01F42D6}"/>
+    <hyperlink ref="C7" r:id="rId15" xr:uid="{B031A56D-0134-5743-B129-001728B0104E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Reverse Words in a String III  Two pointers solution
</commit_message>
<xml_diff>
--- a/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
+++ b/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamal/Documents/yallafix/leecode-java/src/main/java/org/code/challenges/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B14F95-64AF-4D49-A4E8-D8BBB9AA2B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31477D8-6B9E-F04C-89C4-1F05BD2105C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
   <si>
     <t>Category</t>
   </si>
@@ -659,6 +659,22 @@
         <rFont val="Arial (Body)"/>
       </rPr>
       <t xml:space="preserve"> (if ((strIndex == s.length() - 1) || s.charAt(strIndex) == ' ')) </t>
+    </r>
+  </si>
+  <si>
+    <t>ReverseWordsInAStringIII_TwoPointers</t>
+  </si>
+  <si>
+    <r>
+      <t>Two poiners : Copy all strings to char[] and swap lastIndex with startIndex and have two pointers the decreases and increment in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> while loop  </t>
     </r>
   </si>
 </sst>
@@ -1018,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13703DB-FEA8-9246-9D4D-5D4B2C6A9445}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1149,13 +1165,13 @@
         <v>68</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1163,39 +1179,39 @@
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.2">
@@ -1209,44 +1225,50 @@
         <v>57</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>27</v>
+      <c r="B12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1254,10 +1276,10 @@
         <v>3</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>26</v>
@@ -1268,16 +1290,13 @@
         <v>3</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1285,13 +1304,16 @@
         <v>3</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1299,33 +1321,30 @@
         <v>3</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>31</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>42</v>
+        <v>31</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1333,24 +1352,24 @@
         <v>39</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>44</v>
@@ -1359,26 +1378,43 @@
         <v>45</v>
       </c>
       <c r="F19" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="19" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="12" t="s">
+    <row r="21" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C21" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E21" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F21" s="8" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1389,16 +1425,17 @@
     <hyperlink ref="C4" r:id="rId3" xr:uid="{6B9C3297-C807-CF43-AA7B-E97378371948}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{2A0E9DC2-E8F4-764A-989D-FBB9493AF002}"/>
     <hyperlink ref="C6" r:id="rId5" xr:uid="{C9094BB3-3FEE-B44C-A115-D650C9CB57A5}"/>
-    <hyperlink ref="C11" r:id="rId6" xr:uid="{B9BEF090-2AFE-9441-AD50-35C1A5966885}"/>
-    <hyperlink ref="C14" r:id="rId7" xr:uid="{F7F388A7-ACD1-E140-B119-D7BCFD50F5FE}"/>
-    <hyperlink ref="C16" r:id="rId8" xr:uid="{77A7E089-AC14-AB4A-B671-C0D310CB6CF3}"/>
-    <hyperlink ref="C17" r:id="rId9" xr:uid="{BCDCDE6F-1466-074A-BB9F-F0CB675CA923}"/>
-    <hyperlink ref="C18" r:id="rId10" xr:uid="{0C111F3E-212C-5649-8472-D8D2118553C9}"/>
-    <hyperlink ref="C19" r:id="rId11" xr:uid="{FA8897B0-989F-4843-8C79-077B8E564DE2}"/>
-    <hyperlink ref="C8" r:id="rId12" xr:uid="{1ED9A352-B7B9-AB40-B432-CF109BDAF648}"/>
-    <hyperlink ref="C10" r:id="rId13" xr:uid="{AAA3065A-A5DD-DA4B-B0C7-BB17201B4434}"/>
-    <hyperlink ref="C20" r:id="rId14" xr:uid="{6A8EE19C-D739-2B4C-A65D-8F9DF01F42D6}"/>
-    <hyperlink ref="C7" r:id="rId15" xr:uid="{B031A56D-0134-5743-B129-001728B0104E}"/>
+    <hyperlink ref="C12" r:id="rId6" xr:uid="{B9BEF090-2AFE-9441-AD50-35C1A5966885}"/>
+    <hyperlink ref="C15" r:id="rId7" xr:uid="{F7F388A7-ACD1-E140-B119-D7BCFD50F5FE}"/>
+    <hyperlink ref="C17" r:id="rId8" xr:uid="{77A7E089-AC14-AB4A-B671-C0D310CB6CF3}"/>
+    <hyperlink ref="C18" r:id="rId9" xr:uid="{BCDCDE6F-1466-074A-BB9F-F0CB675CA923}"/>
+    <hyperlink ref="C19" r:id="rId10" xr:uid="{0C111F3E-212C-5649-8472-D8D2118553C9}"/>
+    <hyperlink ref="C20" r:id="rId11" xr:uid="{FA8897B0-989F-4843-8C79-077B8E564DE2}"/>
+    <hyperlink ref="C9" r:id="rId12" xr:uid="{1ED9A352-B7B9-AB40-B432-CF109BDAF648}"/>
+    <hyperlink ref="C11" r:id="rId13" xr:uid="{AAA3065A-A5DD-DA4B-B0C7-BB17201B4434}"/>
+    <hyperlink ref="C21" r:id="rId14" xr:uid="{6A8EE19C-D739-2B4C-A65D-8F9DF01F42D6}"/>
+    <hyperlink ref="C8" r:id="rId15" xr:uid="{B031A56D-0134-5743-B129-001728B0104E}"/>
+    <hyperlink ref="C7" r:id="rId16" xr:uid="{D8C68F35-E592-694F-B074-1E28C3DD241D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revers only letters challenge
</commit_message>
<xml_diff>
--- a/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
+++ b/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamal/Documents/yallafix/leecode-java/src/main/java/org/code/challenges/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31477D8-6B9E-F04C-89C4-1F05BD2105C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025CCACA-381F-A34B-83A0-28859216DA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="82">
   <si>
     <t>Category</t>
   </si>
@@ -675,6 +675,71 @@
         <rFont val="Arial (Body)"/>
       </rPr>
       <t xml:space="preserve"> while loop  </t>
+    </r>
+  </si>
+  <si>
+    <t>Reverse Pointer</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-only-letters</t>
+  </si>
+  <si>
+    <t>ReverseOnlyLetters_ReversePointer</t>
+  </si>
+  <si>
+    <t>ReverseOnlyLetters_Stack</t>
+  </si>
+  <si>
+    <t>Stack (Pop, Push)</t>
+  </si>
+  <si>
+    <r>
+      <t>Use</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> Stack </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> Technique (Collect the letters of 'S' separately into a stack, so that popping the stack reverses the letters)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Use</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> Reverse Pointer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> Technique: You need two loop, the first loop will check if the left character can be reversed, if so then we need another loop that will check if right character can be reversed  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> (int j = S.length() - 1;   while (!Character.isLetter(S.charAt(j))) j--)  </t>
     </r>
   </si>
 </sst>
@@ -1034,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13703DB-FEA8-9246-9D4D-5D4B2C6A9445}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1254,49 +1319,61 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>19</v>
+      <c r="B12" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>24</v>
+        <v>76</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>32</v>
+      <c r="B13" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>25</v>
+      <c r="B14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1304,16 +1381,13 @@
         <v>3</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1321,13 +1395,13 @@
         <v>3</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1335,86 +1409,117 @@
         <v>3</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>42</v>
+        <v>31</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E22" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F22" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="19" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="12" t="s">
+    <row r="23" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E23" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F23" s="8" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1425,17 +1530,19 @@
     <hyperlink ref="C4" r:id="rId3" xr:uid="{6B9C3297-C807-CF43-AA7B-E97378371948}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{2A0E9DC2-E8F4-764A-989D-FBB9493AF002}"/>
     <hyperlink ref="C6" r:id="rId5" xr:uid="{C9094BB3-3FEE-B44C-A115-D650C9CB57A5}"/>
-    <hyperlink ref="C12" r:id="rId6" xr:uid="{B9BEF090-2AFE-9441-AD50-35C1A5966885}"/>
-    <hyperlink ref="C15" r:id="rId7" xr:uid="{F7F388A7-ACD1-E140-B119-D7BCFD50F5FE}"/>
-    <hyperlink ref="C17" r:id="rId8" xr:uid="{77A7E089-AC14-AB4A-B671-C0D310CB6CF3}"/>
-    <hyperlink ref="C18" r:id="rId9" xr:uid="{BCDCDE6F-1466-074A-BB9F-F0CB675CA923}"/>
-    <hyperlink ref="C19" r:id="rId10" xr:uid="{0C111F3E-212C-5649-8472-D8D2118553C9}"/>
-    <hyperlink ref="C20" r:id="rId11" xr:uid="{FA8897B0-989F-4843-8C79-077B8E564DE2}"/>
+    <hyperlink ref="C14" r:id="rId6" xr:uid="{B9BEF090-2AFE-9441-AD50-35C1A5966885}"/>
+    <hyperlink ref="C17" r:id="rId7" xr:uid="{F7F388A7-ACD1-E140-B119-D7BCFD50F5FE}"/>
+    <hyperlink ref="C19" r:id="rId8" xr:uid="{77A7E089-AC14-AB4A-B671-C0D310CB6CF3}"/>
+    <hyperlink ref="C20" r:id="rId9" xr:uid="{BCDCDE6F-1466-074A-BB9F-F0CB675CA923}"/>
+    <hyperlink ref="C21" r:id="rId10" xr:uid="{0C111F3E-212C-5649-8472-D8D2118553C9}"/>
+    <hyperlink ref="C22" r:id="rId11" xr:uid="{FA8897B0-989F-4843-8C79-077B8E564DE2}"/>
     <hyperlink ref="C9" r:id="rId12" xr:uid="{1ED9A352-B7B9-AB40-B432-CF109BDAF648}"/>
     <hyperlink ref="C11" r:id="rId13" xr:uid="{AAA3065A-A5DD-DA4B-B0C7-BB17201B4434}"/>
-    <hyperlink ref="C21" r:id="rId14" xr:uid="{6A8EE19C-D739-2B4C-A65D-8F9DF01F42D6}"/>
+    <hyperlink ref="C23" r:id="rId14" xr:uid="{6A8EE19C-D739-2B4C-A65D-8F9DF01F42D6}"/>
     <hyperlink ref="C8" r:id="rId15" xr:uid="{B031A56D-0134-5743-B129-001728B0104E}"/>
     <hyperlink ref="C7" r:id="rId16" xr:uid="{D8C68F35-E592-694F-B074-1E28C3DD241D}"/>
+    <hyperlink ref="C13" r:id="rId17" xr:uid="{A1684345-5477-0F4D-95A7-DF38E28D89B8}"/>
+    <hyperlink ref="C12" r:id="rId18" xr:uid="{F400BD3C-697A-EC4A-9115-6AAAF80D3EC7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Hashing TwoSum and FirstLetterToAppear
</commit_message>
<xml_diff>
--- a/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
+++ b/src/main/java/org/code/challenges/leetcode/Leetcode _75_Questions_Nots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamal/Documents/yallafix/leecode-java/src/main/java/org/code/challenges/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025CCACA-381F-A34B-83A0-28859216DA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FBD3AE-0D3E-0A4A-BB1E-9EC9EF8BE15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="91">
   <si>
     <t>Category</t>
   </si>
@@ -740,6 +740,63 @@
         <rFont val="Arial (Body)"/>
       </rPr>
       <t xml:space="preserve"> (int j = S.length() - 1;   while (!Character.isLetter(S.charAt(j))) j--)  </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Hashing </t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/first-letter-to-appear-twice</t>
+  </si>
+  <si>
+    <t>First Letter to Appear Twice</t>
+  </si>
+  <si>
+    <t>FirstLetterToAppearTwice</t>
+  </si>
+  <si>
+    <t>Data Structure (Set)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="5"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve">Set: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t>Use set to store seen characters</t>
+    </r>
+  </si>
+  <si>
+    <t>TwoSum_HashTable</t>
+  </si>
+  <si>
+    <t>Data Structure (HashMap)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve">HashMap: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t>Use HashMap to store values and use this formula to check whether sum of target contains in Map  (target - nums[i];)</t>
     </r>
   </si>
 </sst>
@@ -747,7 +804,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -802,6 +859,19 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial (Body)"/>
     </font>
   </fonts>
   <fills count="4">
@@ -865,7 +935,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -882,6 +952,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1099,15 +1175,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13703DB-FEA8-9246-9D4D-5D4B2C6A9445}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="54.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="54.6640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="63.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65.5" style="3" customWidth="1"/>
     <col min="5" max="5" width="76.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -1523,7 +1600,58 @@
         <v>66</v>
       </c>
     </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A26:D26"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{0AFF85C1-CA37-F747-8CE3-0D0C9E7AC2A0}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{367ADF6A-5F17-A346-9DDF-ABD931F11AF9}"/>
@@ -1543,6 +1671,8 @@
     <hyperlink ref="C7" r:id="rId16" xr:uid="{D8C68F35-E592-694F-B074-1E28C3DD241D}"/>
     <hyperlink ref="C13" r:id="rId17" xr:uid="{A1684345-5477-0F4D-95A7-DF38E28D89B8}"/>
     <hyperlink ref="C12" r:id="rId18" xr:uid="{F400BD3C-697A-EC4A-9115-6AAAF80D3EC7}"/>
+    <hyperlink ref="C28" r:id="rId19" xr:uid="{46B153E7-4D1E-AD47-B84C-1AC037305EC3}"/>
+    <hyperlink ref="C27" r:id="rId20" xr:uid="{C3A7855B-CF30-764F-8E3A-2F7A2EEF233E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>